<commit_message>
Second commit, added all the batch brs test case with stage 1 and stage 2 validations.
</commit_message>
<xml_diff>
--- a/src/test/resources/clientDetails.xlsx
+++ b/src/test/resources/clientDetails.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Phedora\Eazypayouts\Reco Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830951D0-190C-491E-8399-FFCC68A863CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139BF0B3-2D78-48E9-BB72-B7910C7A2CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Recon TestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="165">
   <si>
     <t>ledger label</t>
   </si>
@@ -295,6 +296,231 @@
   </si>
   <si>
     <t>ESCR0123456</t>
+  </si>
+  <si>
+    <t>utr</t>
+  </si>
+  <si>
+    <t>payout_ref</t>
+  </si>
+  <si>
+    <t>20240628104705GuruLiveImps156</t>
+  </si>
+  <si>
+    <t>418010292157</t>
+  </si>
+  <si>
+    <t>20240628111840GuruLiveUPI068</t>
+  </si>
+  <si>
+    <t>418060636054</t>
+  </si>
+  <si>
+    <t>20240701184240GuruLiveImps157</t>
+  </si>
+  <si>
+    <t>418318534644</t>
+  </si>
+  <si>
+    <t>20240702110814GuruLiveImps158</t>
+  </si>
+  <si>
+    <t>statement not there</t>
+  </si>
+  <si>
+    <t>20240702112004GuruLiveUPI069</t>
+  </si>
+  <si>
+    <t>20240702114451GuruLiveImps159</t>
+  </si>
+  <si>
+    <t>418411492943</t>
+  </si>
+  <si>
+    <t>20240702122011GuruLiveImps160</t>
+  </si>
+  <si>
+    <t>418412694971</t>
+  </si>
+  <si>
+    <t>20240702130310GuruLiveImps161</t>
+  </si>
+  <si>
+    <t>418413948429</t>
+  </si>
+  <si>
+    <t>20240702132024GuruLiveImps162</t>
+  </si>
+  <si>
+    <t>418413047835</t>
+  </si>
+  <si>
+    <t>20240702145931GuruLiveImps163</t>
+  </si>
+  <si>
+    <t>418414593036</t>
+  </si>
+  <si>
+    <t>20240702151958GuruLiveImps164</t>
+  </si>
+  <si>
+    <t>418415710539</t>
+  </si>
+  <si>
+    <t>20240702152757GuruLiveImps165</t>
+  </si>
+  <si>
+    <t>418415753757</t>
+  </si>
+  <si>
+    <t>20240702155416GuruLiveImps166</t>
+  </si>
+  <si>
+    <t>418415897422</t>
+  </si>
+  <si>
+    <t>20240702161244GuruLiveImps167</t>
+  </si>
+  <si>
+    <t>418416998078</t>
+  </si>
+  <si>
+    <t>20240702163247GuruLiveImps168</t>
+  </si>
+  <si>
+    <t>418416109506</t>
+  </si>
+  <si>
+    <t>20240702165316GuruLiveImps169</t>
+  </si>
+  <si>
+    <t>418416222778</t>
+  </si>
+  <si>
+    <t>20240702180711GuruLiveImps170</t>
+  </si>
+  <si>
+    <t>418418660067</t>
+  </si>
+  <si>
+    <t>20240702181818GuruLiveImps171</t>
+  </si>
+  <si>
+    <t>418418727807</t>
+  </si>
+  <si>
+    <t>20240702184023GuruLiveImps172</t>
+  </si>
+  <si>
+    <t>20240702185516GuruLiveImps173</t>
+  </si>
+  <si>
+    <t>418418972949</t>
+  </si>
+  <si>
+    <t>20240703104547GuruLiveImps174</t>
+  </si>
+  <si>
+    <t>418510310393</t>
+  </si>
+  <si>
+    <t>20240703110210GuruLiveImps175</t>
+  </si>
+  <si>
+    <t>418511397426</t>
+  </si>
+  <si>
+    <t>20240703110950GuruLiveImps176</t>
+  </si>
+  <si>
+    <t>418511440038</t>
+  </si>
+  <si>
+    <t>20240703111943GuruLiveUPI072</t>
+  </si>
+  <si>
+    <t>418514879410</t>
+  </si>
+  <si>
+    <t>20240716105055GuruLiveImps178</t>
+  </si>
+  <si>
+    <t>419810063628</t>
+  </si>
+  <si>
+    <t>20240716110407GuruLiveImps179</t>
+  </si>
+  <si>
+    <t>419811135076</t>
+  </si>
+  <si>
+    <t>20240716112109GuruLiveImps180</t>
+  </si>
+  <si>
+    <t>419811229667</t>
+  </si>
+  <si>
+    <t>20240716112109GuruLiveImps181</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>20240716115603GuruLiveImps182</t>
+  </si>
+  <si>
+    <t>419811423515</t>
+  </si>
+  <si>
+    <t>20240716124107GuruLiveImps187</t>
+  </si>
+  <si>
+    <t>419812689432</t>
+  </si>
+  <si>
+    <t>20240716120606GuruLiveImps183</t>
+  </si>
+  <si>
+    <t>419812480230</t>
+  </si>
+  <si>
+    <t>20240716121630GuruLiveImps184</t>
+  </si>
+  <si>
+    <t>419812542990</t>
+  </si>
+  <si>
+    <t>20240716122126GuruLiveImps185</t>
+  </si>
+  <si>
+    <t>419812573053</t>
+  </si>
+  <si>
+    <t>20240716123248GuruLiveImps186</t>
+  </si>
+  <si>
+    <t>419812640771</t>
+  </si>
+  <si>
+    <t>20240716124923GuruLiveUPI074</t>
+  </si>
+  <si>
+    <t>419828709383</t>
+  </si>
+  <si>
+    <t>20240716125719GuruLiveUPI075</t>
+  </si>
+  <si>
+    <t>not generated</t>
+  </si>
+  <si>
+    <t>20240716130646GuruLiveUPI076</t>
+  </si>
+  <si>
+    <t>not generateded</t>
+  </si>
+  <si>
+    <t>123456789012</t>
   </si>
 </sst>
 </file>
@@ -336,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -344,6 +570,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1377,4 +1604,405 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B239CD-BA1A-4E12-9EBE-0EFA1EE876BA}">
+  <dimension ref="A1:B49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>152</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>154</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>160</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:B49" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
created classes to get the van collects, payout log and to get the CRN of utr from the payout log given.
</commit_message>
<xml_diff>
--- a/src/test/resources/clientDetails.xlsx
+++ b/src/test/resources/clientDetails.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Phedora\Eazypayouts\Reco Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139BF0B3-2D78-48E9-BB72-B7910C7A2CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44246731-9336-4825-B66D-942CBC699906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bank" sheetId="1" r:id="rId1"/>
     <sheet name="Recon TestData" sheetId="2" r:id="rId2"/>
+    <sheet name="CRN fetch" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="713">
   <si>
     <t>ledger label</t>
   </si>
@@ -521,13 +522,1657 @@
   </si>
   <si>
     <t>123456789012</t>
+  </si>
+  <si>
+    <t>No payout log</t>
+  </si>
+  <si>
+    <t>422618580920,</t>
+  </si>
+  <si>
+    <t>422618584052,</t>
+  </si>
+  <si>
+    <t>422521481610,</t>
+  </si>
+  <si>
+    <t>422521481520,</t>
+  </si>
+  <si>
+    <t>422521495318,</t>
+  </si>
+  <si>
+    <t>422521494698,</t>
+  </si>
+  <si>
+    <t>422521493078,</t>
+  </si>
+  <si>
+    <t>422521481911,</t>
+  </si>
+  <si>
+    <t>422521481991,</t>
+  </si>
+  <si>
+    <t>422521485921,</t>
+  </si>
+  <si>
+    <t>422521490821,</t>
+  </si>
+  <si>
+    <t>422521477968,</t>
+  </si>
+  <si>
+    <t>422521491998,</t>
+  </si>
+  <si>
+    <t>422521481901,</t>
+  </si>
+  <si>
+    <t>422521483071,</t>
+  </si>
+  <si>
+    <t>422521486191,</t>
+  </si>
+  <si>
+    <t>422521491391,</t>
+  </si>
+  <si>
+    <t>422521493851,</t>
+  </si>
+  <si>
+    <t>422521479052,</t>
+  </si>
+  <si>
+    <t>422521483190,</t>
+  </si>
+  <si>
+    <t>422521498720,</t>
+  </si>
+  <si>
+    <t>422521484310,</t>
+  </si>
+  <si>
+    <t>422521493106,</t>
+  </si>
+  <si>
+    <t>422521479288,</t>
+  </si>
+  <si>
+    <t>422521479191,</t>
+  </si>
+  <si>
+    <t>422521483091,</t>
+  </si>
+  <si>
+    <t>422521483391,</t>
+  </si>
+  <si>
+    <t>422521491392,</t>
+  </si>
+  <si>
+    <t>422521480405,</t>
+  </si>
+  <si>
+    <t>422521478991,</t>
+  </si>
+  <si>
+    <t>422521478911,</t>
+  </si>
+  <si>
+    <t>422521490832,</t>
+  </si>
+  <si>
+    <t>422521489583,</t>
+  </si>
+  <si>
+    <t>422521501005,</t>
+  </si>
+  <si>
+    <t>422521483790,</t>
+  </si>
+  <si>
+    <t>422521484520,</t>
+  </si>
+  <si>
+    <t>422521481227,</t>
+  </si>
+  <si>
+    <t>422521495335,</t>
+  </si>
+  <si>
+    <t>422521485380,</t>
+  </si>
+  <si>
+    <t>422521483296,</t>
+  </si>
+  <si>
+    <t>422521483086,</t>
+  </si>
+  <si>
+    <t>422521495329,</t>
+  </si>
+  <si>
+    <t>422521486931,</t>
+  </si>
+  <si>
+    <t>422521483491,</t>
+  </si>
+  <si>
+    <t>422521492241,</t>
+  </si>
+  <si>
+    <t>422521491911,</t>
+  </si>
+  <si>
+    <t>422521490912,</t>
+  </si>
+  <si>
+    <t>422521491502,</t>
+  </si>
+  <si>
+    <t>422521492242,</t>
+  </si>
+  <si>
+    <t>422521492082,</t>
+  </si>
+  <si>
+    <t>422521491832,</t>
+  </si>
+  <si>
+    <t>422521493854,</t>
+  </si>
+  <si>
+    <t>422521484145,</t>
+  </si>
+  <si>
+    <t>422521483585,</t>
+  </si>
+  <si>
+    <t>422521483495,</t>
+  </si>
+  <si>
+    <t>422521484455,</t>
+  </si>
+  <si>
+    <t>422521491665,</t>
+  </si>
+  <si>
+    <t>422521491692,</t>
+  </si>
+  <si>
+    <t>422521492152,</t>
+  </si>
+  <si>
+    <t>422521492155,</t>
+  </si>
+  <si>
+    <t>422521499057,</t>
+  </si>
+  <si>
+    <t>422521491762,</t>
+  </si>
+  <si>
+    <t>422521492978,</t>
+  </si>
+  <si>
+    <t>422521489208,</t>
+  </si>
+  <si>
+    <t>422521485051,</t>
+  </si>
+  <si>
+    <t>422521485061,</t>
+  </si>
+  <si>
+    <t>422521478413,</t>
+  </si>
+  <si>
+    <t>422521491663,</t>
+  </si>
+  <si>
+    <t>422521491763,</t>
+  </si>
+  <si>
+    <t>422521491753,</t>
+  </si>
+  <si>
+    <t>422521484785,</t>
+  </si>
+  <si>
+    <t>422521485205,</t>
+  </si>
+  <si>
+    <t>422521485225,</t>
+  </si>
+  <si>
+    <t>422521488475,</t>
+  </si>
+  <si>
+    <t>422521484386,</t>
+  </si>
+  <si>
+    <t>422521495246,</t>
+  </si>
+  <si>
+    <t>422521494366,</t>
+  </si>
+  <si>
+    <t>422521499476,</t>
+  </si>
+  <si>
+    <t>422521483187,</t>
+  </si>
+  <si>
+    <t>422521479978,</t>
+  </si>
+  <si>
+    <t>422521485081,</t>
+  </si>
+  <si>
+    <t>422521492982,</t>
+  </si>
+  <si>
+    <t>422521482977,</t>
+  </si>
+  <si>
+    <t>422521498158,</t>
+  </si>
+  <si>
+    <t>422521485211,</t>
+  </si>
+  <si>
+    <t>422521484971,</t>
+  </si>
+  <si>
+    <t>422521493184,</t>
+  </si>
+  <si>
+    <t>422521485226,</t>
+  </si>
+  <si>
+    <t>422521483886,</t>
+  </si>
+  <si>
+    <t>422521485066,</t>
+  </si>
+  <si>
+    <t>422521484457,</t>
+  </si>
+  <si>
+    <t>422521484397,</t>
+  </si>
+  <si>
+    <t>422521491917,</t>
+  </si>
+  <si>
+    <t>422521501007,</t>
+  </si>
+  <si>
+    <t>422521496679,</t>
+  </si>
+  <si>
+    <t>422521478713,</t>
+  </si>
+  <si>
+    <t>422521477955,</t>
+  </si>
+  <si>
+    <t>422521481914,</t>
+  </si>
+  <si>
+    <t>422521484025,</t>
+  </si>
+  <si>
+    <t>422521485586,</t>
+  </si>
+  <si>
+    <t>422521486236,</t>
+  </si>
+  <si>
+    <t>422521486336,</t>
+  </si>
+  <si>
+    <t>422521484537,</t>
+  </si>
+  <si>
+    <t>422521485187,</t>
+  </si>
+  <si>
+    <t>422521485367,</t>
+  </si>
+  <si>
+    <t>422521485397,</t>
+  </si>
+  <si>
+    <t>422521477949,</t>
+  </si>
+  <si>
+    <t>422521478589,</t>
+  </si>
+  <si>
+    <t>422521478412,</t>
+  </si>
+  <si>
+    <t>422521485487,</t>
+  </si>
+  <si>
+    <t>422521480092,</t>
+  </si>
+  <si>
+    <t>422521478914,</t>
+  </si>
+  <si>
+    <t>422521479294,</t>
+  </si>
+  <si>
+    <t>422521483084,</t>
+  </si>
+  <si>
+    <t>422521482904,</t>
+  </si>
+  <si>
+    <t>422521491834,</t>
+  </si>
+  <si>
+    <t>422521487266,</t>
+  </si>
+  <si>
+    <t>422521484816,</t>
+  </si>
+  <si>
+    <t>422521485597,</t>
+  </si>
+  <si>
+    <t>422521485216,</t>
+  </si>
+  <si>
+    <t>422521487366,</t>
+  </si>
+  <si>
+    <t>422521486337,</t>
+  </si>
+  <si>
+    <t>422521486417,</t>
+  </si>
+  <si>
+    <t>422521481868,</t>
+  </si>
+  <si>
+    <t>422521494371,</t>
+  </si>
+  <si>
+    <t>422521481332,</t>
+  </si>
+  <si>
+    <t>422521481982,</t>
+  </si>
+  <si>
+    <t>422521479103,</t>
+  </si>
+  <si>
+    <t>422521480283,</t>
+  </si>
+  <si>
+    <t>422521493523,</t>
+  </si>
+  <si>
+    <t>422521497324,</t>
+  </si>
+  <si>
+    <t>422521487377,</t>
+  </si>
+  <si>
+    <t>422521479279,</t>
+  </si>
+  <si>
+    <t>422521480079,</t>
+  </si>
+  <si>
+    <t>422521483379,</t>
+  </si>
+  <si>
+    <t>422521483289,</t>
+  </si>
+  <si>
+    <t>422521484801,</t>
+  </si>
+  <si>
+    <t>422521483582,</t>
+  </si>
+  <si>
+    <t>422521493622,</t>
+  </si>
+  <si>
+    <t>422521483384,</t>
+  </si>
+  <si>
+    <t>422521483492,</t>
+  </si>
+  <si>
+    <t>422521483702,</t>
+  </si>
+  <si>
+    <t>422521480294,</t>
+  </si>
+  <si>
+    <t>422521483294,</t>
+  </si>
+  <si>
+    <t>422521482974,</t>
+  </si>
+  <si>
+    <t>422521484064,</t>
+  </si>
+  <si>
+    <t>422521484214,</t>
+  </si>
+  <si>
+    <t>422521485494,</t>
+  </si>
+  <si>
+    <t>422521480815,</t>
+  </si>
+  <si>
+    <t>422521478395,</t>
+  </si>
+  <si>
+    <t>422521477876,</t>
+  </si>
+  <si>
+    <t>422521478776,</t>
+  </si>
+  <si>
+    <t>422521478986,</t>
+  </si>
+  <si>
+    <t>422521479106,</t>
+  </si>
+  <si>
+    <t>422521488486,</t>
+  </si>
+  <si>
+    <t>422521489216,</t>
+  </si>
+  <si>
+    <t>422521491699,</t>
+  </si>
+  <si>
+    <t>422521491849,</t>
+  </si>
+  <si>
+    <t>422521491839,</t>
+  </si>
+  <si>
+    <t>422521491999,</t>
+  </si>
+  <si>
+    <t>422521482978,</t>
+  </si>
+  <si>
+    <t>422521483722,</t>
+  </si>
+  <si>
+    <t>422521483982,</t>
+  </si>
+  <si>
+    <t>422521485082,</t>
+  </si>
+  <si>
+    <t>422521486045,</t>
+  </si>
+  <si>
+    <t>422521479036,</t>
+  </si>
+  <si>
+    <t>422521493079,</t>
+  </si>
+  <si>
+    <t>422521483792,</t>
+  </si>
+  <si>
+    <t>422521486344,</t>
+  </si>
+  <si>
+    <t>422521484622,</t>
+  </si>
+  <si>
+    <t>422521485685,</t>
+  </si>
+  <si>
+    <t>422521485585,</t>
+  </si>
+  <si>
+    <t>422521480176,</t>
+  </si>
+  <si>
+    <t>422521496961,</t>
+  </si>
+  <si>
+    <t>422521478585,</t>
+  </si>
+  <si>
+    <t>422521478685,</t>
+  </si>
+  <si>
+    <t>422521478507,</t>
+  </si>
+  <si>
+    <t>422521491397,</t>
+  </si>
+  <si>
+    <t>422521480599,</t>
+  </si>
+  <si>
+    <t>422521483799,</t>
+  </si>
+  <si>
+    <t>422521492399,</t>
+  </si>
+  <si>
+    <t>422521497903,</t>
+  </si>
+  <si>
+    <t>422521481893,</t>
+  </si>
+  <si>
+    <t>422521482823,</t>
+  </si>
+  <si>
+    <t>422521497904,</t>
+  </si>
+  <si>
+    <t>422521484534,</t>
+  </si>
+  <si>
+    <t>422521484614,</t>
+  </si>
+  <si>
+    <t>422521486345,</t>
+  </si>
+  <si>
+    <t>422521487285,</t>
+  </si>
+  <si>
+    <t>422521481216,</t>
+  </si>
+  <si>
+    <t>422521490906,</t>
+  </si>
+  <si>
+    <t>422521486598,</t>
+  </si>
+  <si>
+    <t>422521483608,</t>
+  </si>
+  <si>
+    <t>422521484208,</t>
+  </si>
+  <si>
+    <t>422521484458,</t>
+  </si>
+  <si>
+    <t>422521492064,</t>
+  </si>
+  <si>
+    <t>422521484313,</t>
+  </si>
+  <si>
+    <t>422521483643,</t>
+  </si>
+  <si>
+    <t>422521484383,</t>
+  </si>
+  <si>
+    <t>422521479973,</t>
+  </si>
+  <si>
+    <t>422521482043,</t>
+  </si>
+  <si>
+    <t>422521483085,</t>
+  </si>
+  <si>
+    <t>422521478775,</t>
+  </si>
+  <si>
+    <t>422521478795,</t>
+  </si>
+  <si>
+    <t>422521484065,</t>
+  </si>
+  <si>
+    <t>422521482905,</t>
+  </si>
+  <si>
+    <t>422521487075,</t>
+  </si>
+  <si>
+    <t>422521478500,</t>
+  </si>
+  <si>
+    <t>422521478700,</t>
+  </si>
+  <si>
+    <t>422521480080,</t>
+  </si>
+  <si>
+    <t>422521490730,</t>
+  </si>
+  <si>
+    <t>422521491570,</t>
+  </si>
+  <si>
+    <t>422521479180,</t>
+  </si>
+  <si>
+    <t>422521492396,</t>
+  </si>
+  <si>
+    <t>422521487275,</t>
+  </si>
+  <si>
+    <t>422521490650,</t>
+  </si>
+  <si>
+    <t>422521490740,</t>
+  </si>
+  <si>
+    <t>422521485089,</t>
+  </si>
+  <si>
+    <t>422521484799,</t>
+  </si>
+  <si>
+    <t>422521483878,</t>
+  </si>
+  <si>
+    <t>422521485552,</t>
+  </si>
+  <si>
+    <t>422521483983,</t>
+  </si>
+  <si>
+    <t>422521478694,</t>
+  </si>
+  <si>
+    <t>422521477804,</t>
+  </si>
+  <si>
+    <t>422521483295,</t>
+  </si>
+  <si>
+    <t>422521478710,</t>
+  </si>
+  <si>
+    <t>422521489409,</t>
+  </si>
+  <si>
+    <t>422521492829,</t>
+  </si>
+  <si>
+    <t>422521485392,</t>
+  </si>
+  <si>
+    <t>422521498843,</t>
+  </si>
+  <si>
+    <t>422521483373,</t>
+  </si>
+  <si>
+    <t>422521485073,</t>
+  </si>
+  <si>
+    <t>422521481794,</t>
+  </si>
+  <si>
+    <t>422521479190,</t>
+  </si>
+  <si>
+    <t>422521493010,</t>
+  </si>
+  <si>
+    <t>422521491830,</t>
+  </si>
+  <si>
+    <t>422521491990,</t>
+  </si>
+  <si>
+    <t>422521485489,</t>
+  </si>
+  <si>
+    <t>422521487574,</t>
+  </si>
+  <si>
+    <t>422521491920,</t>
+  </si>
+  <si>
+    <t>422521481519,</t>
+  </si>
+  <si>
+    <t>422521486439,</t>
+  </si>
+  <si>
+    <t>422521486432,</t>
+  </si>
+  <si>
+    <t>422521485692,</t>
+  </si>
+  <si>
+    <t>422521485373,</t>
+  </si>
+  <si>
+    <t>422521485543,</t>
+  </si>
+  <si>
+    <t>422521486193,</t>
+  </si>
+  <si>
+    <t>422521490734,</t>
+  </si>
+  <si>
+    <t>422521485812,</t>
+  </si>
+  <si>
+    <t>422521492500,</t>
+  </si>
+  <si>
+    <t>422521493080,</t>
+  </si>
+  <si>
+    <t>422521479650,</t>
+  </si>
+  <si>
+    <t>422521477647,</t>
+  </si>
+  <si>
+    <t>422521477797,</t>
+  </si>
+  <si>
+    <t>422521490907,</t>
+  </si>
+  <si>
+    <t>422521485698,</t>
+  </si>
+  <si>
+    <t>422521491487,</t>
+  </si>
+  <si>
+    <t>422521490818,</t>
+  </si>
+  <si>
+    <t>422521485488,</t>
+  </si>
+  <si>
+    <t>422521489869,</t>
+  </si>
+  <si>
+    <t>422521487282,</t>
+  </si>
+  <si>
+    <t>422521491773,</t>
+  </si>
+  <si>
+    <t>422521492503,</t>
+  </si>
+  <si>
+    <t>422521497090,</t>
+  </si>
+  <si>
+    <t>422521479117,</t>
+  </si>
+  <si>
+    <t>422521479047,</t>
+  </si>
+  <si>
+    <t>422521491997,</t>
+  </si>
+  <si>
+    <t>422521493007,</t>
+  </si>
+  <si>
+    <t>422521477641,</t>
+  </si>
+  <si>
+    <t>422521477711,</t>
+  </si>
+  <si>
+    <t>422521478601,</t>
+  </si>
+  <si>
+    <t>422521488632,</t>
+  </si>
+  <si>
+    <t>422521498395,</t>
+  </si>
+  <si>
+    <t>422614620767,</t>
+  </si>
+  <si>
+    <t>422620544343,</t>
+  </si>
+  <si>
+    <t>422619084137</t>
+  </si>
+  <si>
+    <t>B9YIMVgbBLd</t>
+  </si>
+  <si>
+    <t>B9YIMVgYBLc</t>
+  </si>
+  <si>
+    <t>B9YIMVi1BOt</t>
+  </si>
+  <si>
+    <t>B9YIMVi3BOv</t>
+  </si>
+  <si>
+    <t>B9YIMViXBOd</t>
+  </si>
+  <si>
+    <t>B9YIMVggBLf</t>
+  </si>
+  <si>
+    <t>B9YIMVgiBLk</t>
+  </si>
+  <si>
+    <t>B9YIMVhLBNT</t>
+  </si>
+  <si>
+    <t>B9YIMViHBNw</t>
+  </si>
+  <si>
+    <t>B9YIMVfxBKy</t>
+  </si>
+  <si>
+    <t>B9YIMViUBOV</t>
+  </si>
+  <si>
+    <t>B9YIMVggBLh</t>
+  </si>
+  <si>
+    <t>B9YIMVglBLs</t>
+  </si>
+  <si>
+    <t>B9YIMVhIBNK</t>
+  </si>
+  <si>
+    <t>B9YIMViGBNs</t>
+  </si>
+  <si>
+    <t>B9YIMVioBOn</t>
+  </si>
+  <si>
+    <t>B9YIMVf1BK7</t>
+  </si>
+  <si>
+    <t>B9YIMVgmBLv</t>
+  </si>
+  <si>
+    <t>B9YIMVjgBO6</t>
+  </si>
+  <si>
+    <t>B9YIMVgvBMN</t>
+  </si>
+  <si>
+    <t>B9YIMViXBOe</t>
+  </si>
+  <si>
+    <t>B9YIMVf7BLN</t>
+  </si>
+  <si>
+    <t>B9YIMVf4BLF</t>
+  </si>
+  <si>
+    <t>B9YIMVgkBLq</t>
+  </si>
+  <si>
+    <t>B9YIMVgpBL7</t>
+  </si>
+  <si>
+    <t>B9YIMViHBNu</t>
+  </si>
+  <si>
+    <t>B9YIMVgDBLR</t>
+  </si>
+  <si>
+    <t>B9YIMVf2BLA</t>
+  </si>
+  <si>
+    <t>B9YIMVfzBK5</t>
+  </si>
+  <si>
+    <t>B9YIMViJBN1</t>
+  </si>
+  <si>
+    <t>B9YIMVhxBNn</t>
+  </si>
+  <si>
+    <t>B9YIMVj2BO9</t>
+  </si>
+  <si>
+    <t>B9YIMVgyBMX</t>
+  </si>
+  <si>
+    <t>B9YIMVg2BMd</t>
+  </si>
+  <si>
+    <t>B9YIMVgRBLY</t>
+  </si>
+  <si>
+    <t>B9YIMVi1BOu</t>
+  </si>
+  <si>
+    <t>B9YIMVhCBM5</t>
+  </si>
+  <si>
+    <t>B9YIMVgpBL6</t>
+  </si>
+  <si>
+    <t>B9YIMVgjBLn</t>
+  </si>
+  <si>
+    <t>B9YIMVi1BOs</t>
+  </si>
+  <si>
+    <t>B9YIMVhYBNf</t>
+  </si>
+  <si>
+    <t>B9YIMVgrBMC</t>
+  </si>
+  <si>
+    <t>B9YIMViTBOR</t>
+  </si>
+  <si>
+    <t>B9YIMViTBOQ</t>
+  </si>
+  <si>
+    <t>B9YIMViLBN5</t>
+  </si>
+  <si>
+    <t>B9YIMViIBNy</t>
+  </si>
+  <si>
+    <t>B9YIMViSBOO</t>
+  </si>
+  <si>
+    <t>B9YIMViOBOD</t>
+  </si>
+  <si>
+    <t>B9YIMViPBOG</t>
+  </si>
+  <si>
+    <t>B9YIMVioBOo</t>
+  </si>
+  <si>
+    <t>B9YIMVgrBMB</t>
+  </si>
+  <si>
+    <t>B9YIMVguBMK</t>
+  </si>
+  <si>
+    <t>B9YIMVgsBME</t>
+  </si>
+  <si>
+    <t>B9YIMVgzBMZ</t>
+  </si>
+  <si>
+    <t>B9YIMViMBN7</t>
+  </si>
+  <si>
+    <t>B9YIMViNBN9</t>
+  </si>
+  <si>
+    <t>B9YIMViQBOH</t>
+  </si>
+  <si>
+    <t>B9YIMViRBOM</t>
+  </si>
+  <si>
+    <t>B9YIMVjeBO5</t>
+  </si>
+  <si>
+    <t>B9YIMViOBOC</t>
+  </si>
+  <si>
+    <t>B9YIMVikBOm</t>
+  </si>
+  <si>
+    <t>B9YIMVhoBNk</t>
+  </si>
+  <si>
+    <t>B9YIMVg5BMm</t>
+  </si>
+  <si>
+    <t>B9YIMVg6BMq</t>
+  </si>
+  <si>
+    <t>B9YIMVfqBKe</t>
+  </si>
+  <si>
+    <t>B9YIMViNBN8</t>
+  </si>
+  <si>
+    <t>B9YIMViPBOF</t>
+  </si>
+  <si>
+    <t>B9YIMViNBOB</t>
+  </si>
+  <si>
+    <t>B9YIMVg8BMu</t>
+  </si>
+  <si>
+    <t>B9YIMVg8BMv</t>
+  </si>
+  <si>
+    <t>B9YIMVhBBM1</t>
+  </si>
+  <si>
+    <t>B9YIMVhkBNh</t>
+  </si>
+  <si>
+    <t>B9YIMVgwBMQ</t>
+  </si>
+  <si>
+    <t>B9YIMViyBOr</t>
+  </si>
+  <si>
+    <t>B9YIMVitBOp</t>
+  </si>
+  <si>
+    <t>B9YIMVjoBO8</t>
+  </si>
+  <si>
+    <t>B9YIMVgmBLx</t>
+  </si>
+  <si>
+    <t>B9YIMVgOBLV</t>
+  </si>
+  <si>
+    <t>B9YIMVg5BMn</t>
+  </si>
+  <si>
+    <t>B9YIMVikBOl</t>
+  </si>
+  <si>
+    <t>B9YIMVglBLu</t>
+  </si>
+  <si>
+    <t>B9YIMVjXBO1</t>
+  </si>
+  <si>
+    <t>B9YIMVhBBMz</t>
+  </si>
+  <si>
+    <t>B9YIMVhCBM4</t>
+  </si>
+  <si>
+    <t>B9YIMViXBOf</t>
+  </si>
+  <si>
+    <t>B9YIMVhABMw</t>
+  </si>
+  <si>
+    <t>B9YIMVg1BMb</t>
+  </si>
+  <si>
+    <t>B9YIMVg6BMp</t>
+  </si>
+  <si>
+    <t>B9YIMVgyBMW</t>
+  </si>
+  <si>
+    <t>B9YIMVgxBMS</t>
+  </si>
+  <si>
+    <t>B9YIMViSBOP</t>
+  </si>
+  <si>
+    <t>B9YIMVj3BPA</t>
+  </si>
+  <si>
+    <t>B9YIMVjMBOx</t>
+  </si>
+  <si>
+    <t>B9YIMVfxBKx</t>
+  </si>
+  <si>
+    <t>B9YIMVfyBK2</t>
+  </si>
+  <si>
+    <t>B9YIMVghBLj</t>
+  </si>
+  <si>
+    <t>B9YIMVgoBL3</t>
+  </si>
+  <si>
+    <t>B9YIMVhHBNH</t>
+  </si>
+  <si>
+    <t>B9YIMVhJBNN</t>
+  </si>
+  <si>
+    <t>B9YIMVhLBNR</t>
+  </si>
+  <si>
+    <t>B9YIMVgzBMa</t>
+  </si>
+  <si>
+    <t>B9YIMVg7BMt</t>
+  </si>
+  <si>
+    <t>B9YIMVhDBM7</t>
+  </si>
+  <si>
+    <t>B9YIMVhDBM6</t>
+  </si>
+  <si>
+    <t>B9YIMVfxBKz</t>
+  </si>
+  <si>
+    <t>B9YIMVfvBKq</t>
+  </si>
+  <si>
+    <t>B9YIMVfrBKg</t>
+  </si>
+  <si>
+    <t>B9YIMVhEBM9</t>
+  </si>
+  <si>
+    <t>B9YIMVf5BLH</t>
+  </si>
+  <si>
+    <t>B9YIMVf2BK8</t>
+  </si>
+  <si>
+    <t>B9YIMVf6BLL</t>
+  </si>
+  <si>
+    <t>B9YIMVgkBLp</t>
+  </si>
+  <si>
+    <t>B9YIMVgkBLr</t>
+  </si>
+  <si>
+    <t>B9YIMViQBOJ</t>
+  </si>
+  <si>
+    <t>B9YIMVhTBNa</t>
+  </si>
+  <si>
+    <t>B9YIMVhABMx</t>
+  </si>
+  <si>
+    <t>B9YIMVhGBNF</t>
+  </si>
+  <si>
+    <t>B9YIMVhABMy</t>
+  </si>
+  <si>
+    <t>B9YIMVhWBNd</t>
+  </si>
+  <si>
+    <t>B9YIMVhKBNP</t>
+  </si>
+  <si>
+    <t>B9YIMVhMBNV</t>
+  </si>
+  <si>
+    <t>B9YIMVggBLg</t>
+  </si>
+  <si>
+    <t>B9YIMViuBOq</t>
+  </si>
+  <si>
+    <t>B9YIMVgTBLa</t>
+  </si>
+  <si>
+    <t>B9YIMVgjBLl</t>
+  </si>
+  <si>
+    <t>B9YIMVf3BLD</t>
+  </si>
+  <si>
+    <t>B9YIMVgBBLQ</t>
+  </si>
+  <si>
+    <t>B9YIMVigBOi</t>
+  </si>
+  <si>
+    <t>B9YIMVjMBOy</t>
+  </si>
+  <si>
+    <t>B9YIMVhWBNe</t>
+  </si>
+  <si>
+    <t>B9YIMVf7BLM</t>
+  </si>
+  <si>
+    <t>B9YIMVf6BLK</t>
+  </si>
+  <si>
+    <t>B9YIMVgqBL8</t>
+  </si>
+  <si>
+    <t>B9YIMVgnBLz</t>
+  </si>
+  <si>
+    <t>B9YIMVg7BMs</t>
+  </si>
+  <si>
+    <t>B9YIMVguBML</t>
+  </si>
+  <si>
+    <t>B9YIMVijBOk</t>
+  </si>
+  <si>
+    <t>B9YIMVgqBMA</t>
+  </si>
+  <si>
+    <t>B9YIMVgsBMD</t>
+  </si>
+  <si>
+    <t>B9YIMVgxBMT</t>
+  </si>
+  <si>
+    <t>B9YIMVgABLP</t>
+  </si>
+  <si>
+    <t>B9YIMVgoBL2</t>
+  </si>
+  <si>
+    <t>B9YIMVgnBLy</t>
+  </si>
+  <si>
+    <t>B9YIMVgoBL4</t>
+  </si>
+  <si>
+    <t>B9YIMVgsBMF</t>
+  </si>
+  <si>
+    <t>B9YIMVhEBNB</t>
+  </si>
+  <si>
+    <t>B9YIMVgKBLU</t>
+  </si>
+  <si>
+    <t>B9YIMVfqBKf</t>
+  </si>
+  <si>
+    <t>B9YIMVfvBKs</t>
+  </si>
+  <si>
+    <t>B9YIMVfzBK4</t>
+  </si>
+  <si>
+    <t>B9YIMVf4BLE</t>
+  </si>
+  <si>
+    <t>B9YIMVf3BLC</t>
+  </si>
+  <si>
+    <t>B9YIMVhkBNi</t>
+  </si>
+  <si>
+    <t>B9YIMVhoBNl</t>
+  </si>
+  <si>
+    <t>B9YIMViLBN6</t>
+  </si>
+  <si>
+    <t>B9YIMViRBOL</t>
+  </si>
+  <si>
+    <t>B9YIMViRBOK</t>
+  </si>
+  <si>
+    <t>B9YIMViVBOX</t>
+  </si>
+  <si>
+    <t>B9YIMVgmBLw</t>
+  </si>
+  <si>
+    <t>B9YIMVgwBMO</t>
+  </si>
+  <si>
+    <t>B9YIMVg2BMf</t>
+  </si>
+  <si>
+    <t>B9YIMVg5BMl</t>
+  </si>
+  <si>
+    <t>B9YIMVhDBM8</t>
+  </si>
+  <si>
+    <t>B9YIMVf1BK6</t>
+  </si>
+  <si>
+    <t>B9YIMViWBOb</t>
+  </si>
+  <si>
+    <t>B9YIMVgzBMY</t>
+  </si>
+  <si>
+    <t>B9YIMVhLBNS</t>
+  </si>
+  <si>
+    <t>B9YIMVg3BMh</t>
+  </si>
+  <si>
+    <t>B9YIMVhJBNM</t>
+  </si>
+  <si>
+    <t>B9YIMVhGBNG</t>
+  </si>
+  <si>
+    <t>B9YIMVf7BLO</t>
+  </si>
+  <si>
+    <t>B9YIMVjSBOz</t>
+  </si>
+  <si>
+    <t>B9YIMVfuBKp</t>
+  </si>
+  <si>
+    <t>B9YIMVfwBKu</t>
+  </si>
+  <si>
+    <t>B9YIMVftBKm</t>
+  </si>
+  <si>
+    <t>B9YIMViFBNq</t>
+  </si>
+  <si>
+    <t>B9YIMVgFBLS</t>
+  </si>
+  <si>
+    <t>B9YIMVgxBMU</t>
+  </si>
+  <si>
+    <t>B9YIMViVBOZ</t>
+  </si>
+  <si>
+    <t>B9YIMVjZBO3</t>
+  </si>
+  <si>
+    <t>B9YIMVghBLi</t>
+  </si>
+  <si>
+    <t>B9YIMVgjBLm</t>
+  </si>
+  <si>
+    <t>B9YIMVjZBO2</t>
+  </si>
+  <si>
+    <t>B9YIMVg1BMc</t>
+  </si>
+  <si>
+    <t>B9YIMVg4BMj</t>
+  </si>
+  <si>
+    <t>B9YIMVhKBNQ</t>
+  </si>
+  <si>
+    <t>B9YIMVhUBNc</t>
+  </si>
+  <si>
+    <t>B9YIMVgSBLZ</t>
+  </si>
+  <si>
+    <t>B9YIMViJBN2</t>
+  </si>
+  <si>
+    <t>B9YIMVhRBNY</t>
+  </si>
+  <si>
+    <t>B9YIMVgvBMM</t>
+  </si>
+  <si>
+    <t>B9YIMVgtBMG</t>
+  </si>
+  <si>
+    <t>B9YIMVgyBMV</t>
+  </si>
+  <si>
+    <t>B9YIMViNBOA</t>
+  </si>
+  <si>
+    <t>B9YIMVguBMJ</t>
+  </si>
+  <si>
+    <t>B9YIMVgwBMP</t>
+  </si>
+  <si>
+    <t>B9YIMVgwBMR</t>
+  </si>
+  <si>
+    <t>B9YIMVgPBLW</t>
+  </si>
+  <si>
+    <t>B9YIMVgPBLX</t>
+  </si>
+  <si>
+    <t>B9YIMVgkBLo</t>
+  </si>
+  <si>
+    <t>B9YIMVfzBK3</t>
+  </si>
+  <si>
+    <t>B9YIMVfyBK1</t>
+  </si>
+  <si>
+    <t>B9YIMVgnBL1</t>
+  </si>
+  <si>
+    <t>B9YIMVglBLt</t>
+  </si>
+  <si>
+    <t>B9YIMVhQBNX</t>
+  </si>
+  <si>
+    <t>B9YIMVftBKl</t>
+  </si>
+  <si>
+    <t>B9YIMVfwBKw</t>
+  </si>
+  <si>
+    <t>B9YIMVf5BLI</t>
+  </si>
+  <si>
+    <t>B9YIMViGBNr</t>
+  </si>
+  <si>
+    <t>B9YIMViKBN3</t>
+  </si>
+  <si>
+    <t>B9YIMVf5BLG</t>
+  </si>
+  <si>
+    <t>B9YIMViWBOa</t>
+  </si>
+  <si>
+    <t>B9YIMVhTBNZ</t>
+  </si>
+  <si>
+    <t>B9YIMViEBNp</t>
+  </si>
+  <si>
+    <t>B9YIMViHBNv</t>
+  </si>
+  <si>
+    <t>B9YIMVg6BMo</t>
+  </si>
+  <si>
+    <t>B9YIMVg7BMr</t>
+  </si>
+  <si>
+    <t>B9YIMVg2BMe</t>
+  </si>
+  <si>
+    <t>B9YIMVhFBND</t>
+  </si>
+  <si>
+    <t>B9YIMVg4BMi</t>
+  </si>
+  <si>
+    <t>B9YIMVfvBKt</t>
+  </si>
+  <si>
+    <t>B9YIMVfuBKo</t>
+  </si>
+  <si>
+    <t>B9YIMVgpBL5</t>
+  </si>
+  <si>
+    <t>B9YIMVfwBKv</t>
+  </si>
+  <si>
+    <t>B9YIMVhsBNm</t>
+  </si>
+  <si>
+    <t>B9YIMVihBOj</t>
+  </si>
+  <si>
+    <t>B9YIMVhCBM3</t>
+  </si>
+  <si>
+    <t>B9YIMVjiBO7</t>
+  </si>
+  <si>
+    <t>B9YIMVgqBL9</t>
+  </si>
+  <si>
+    <t>B9YIMVg4BMk</t>
+  </si>
+  <si>
+    <t>B9YIMVgeBLe</t>
+  </si>
+  <si>
+    <t>B9YIMVf6BLJ</t>
+  </si>
+  <si>
+    <t>B9YIMViUBOU</t>
+  </si>
+  <si>
+    <t>B9YIMViQBOI</t>
+  </si>
+  <si>
+    <t>B9YIMViTBOS</t>
+  </si>
+  <si>
+    <t>B9YIMVhEBNA</t>
+  </si>
+  <si>
+    <t>B9YIMVhaBNg</t>
+  </si>
+  <si>
+    <t>B9YIMViSBON</t>
+  </si>
+  <si>
+    <t>B9YIMVgYBLb</t>
+  </si>
+  <si>
+    <t>B9YIMVhMBNU</t>
+  </si>
+  <si>
+    <t>B9YIMVhMBNW</t>
+  </si>
+  <si>
+    <t>B9YIMVhIBNL</t>
+  </si>
+  <si>
+    <t>B9YIMVhBBM2</t>
+  </si>
+  <si>
+    <t>B9YIMVhGBNE</t>
+  </si>
+  <si>
+    <t>B9YIMVhIBNJ</t>
+  </si>
+  <si>
+    <t>B9YIMViGBNt</t>
+  </si>
+  <si>
+    <t>B9YIMVhJBNO</t>
+  </si>
+  <si>
+    <t>B9YIMViYBOh</t>
+  </si>
+  <si>
+    <t>B9YIMViWBOc</t>
+  </si>
+  <si>
+    <t>B9YIMVgGBLT</t>
+  </si>
+  <si>
+    <t>B9YIMVfpBKc</t>
+  </si>
+  <si>
+    <t>B9YIMVftBKn</t>
+  </si>
+  <si>
+    <t>B9YIMViKBN4</t>
+  </si>
+  <si>
+    <t>B9YIMVhHBNI</t>
+  </si>
+  <si>
+    <t>B9YIMViJBNz</t>
+  </si>
+  <si>
+    <t>B9YIMViIBNx</t>
+  </si>
+  <si>
+    <t>B9YIMVhFBNC</t>
+  </si>
+  <si>
+    <t>B9YIMVh3BNo</t>
+  </si>
+  <si>
+    <t>B9YIMVhUBNb</t>
+  </si>
+  <si>
+    <t>B9YIMViOBOE</t>
+  </si>
+  <si>
+    <t>B9YIMViYBOg</t>
+  </si>
+  <si>
+    <t>B9YIMVjFBOw</t>
+  </si>
+  <si>
+    <t>B9YIMVf3BLB</t>
+  </si>
+  <si>
+    <t>B9YIMVf2BK9</t>
+  </si>
+  <si>
+    <t>B9YIMViUBOT</t>
+  </si>
+  <si>
+    <t>B9YIMViUBOW</t>
+  </si>
+  <si>
+    <t>B9YIMVfqBKd</t>
+  </si>
+  <si>
+    <t>B9YIMVfsBKk</t>
+  </si>
+  <si>
+    <t>B9YIMVfvBKr</t>
+  </si>
+  <si>
+    <t>B9YIMVhnBNj</t>
+  </si>
+  <si>
+    <t>B9YIMVjaBO4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +2186,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Droid Sans Mono"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -550,7 +2200,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -558,11 +2208,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -571,6 +2236,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,24 +2525,24 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.21875" customWidth="1"/>
-    <col min="4" max="4" width="51.88671875" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.21875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="51.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="41.6640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -907,7 +2575,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -942,7 +2610,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -977,7 +2645,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1012,7 +2680,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1047,7 +2715,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1082,7 +2750,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1117,7 +2785,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1152,7 +2820,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1187,7 +2855,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1222,7 +2890,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1257,7 +2925,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1272,7 +2940,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1287,7 +2955,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1302,7 +2970,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1317,7 +2985,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1332,7 +3000,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1347,7 +3015,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1362,7 +3030,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1377,7 +3045,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1392,7 +3060,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1406,7 +3074,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1421,7 +3089,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1436,7 +3104,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1451,7 +3119,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1466,7 +3134,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1481,7 +3149,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1496,7 +3164,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1511,7 +3179,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1526,7 +3194,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1541,7 +3209,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1556,7 +3224,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1571,7 +3239,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1586,7 +3254,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1610,17 +3278,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B239CD-BA1A-4E12-9EBE-0EFA1EE876BA}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -1628,7 +3296,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -1636,7 +3304,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -1644,7 +3312,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -1652,7 +3320,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>98</v>
       </c>
@@ -1660,7 +3328,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -1668,12 +3336,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="B7" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1681,7 +3349,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1689,7 +3357,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>103</v>
       </c>
@@ -1697,7 +3365,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -1705,7 +3373,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -1713,7 +3381,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -1721,7 +3389,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>92</v>
       </c>
@@ -1729,7 +3397,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -1737,7 +3405,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -1745,7 +3413,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1753,7 +3421,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>113</v>
       </c>
@@ -1761,7 +3429,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>115</v>
       </c>
@@ -1769,7 +3437,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -1777,7 +3445,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>119</v>
       </c>
@@ -1785,7 +3453,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>121</v>
       </c>
@@ -1793,7 +3461,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>123</v>
       </c>
@@ -1801,7 +3469,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>125</v>
       </c>
@@ -1809,13 +3477,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>127</v>
       </c>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -1823,7 +3491,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1831,7 +3499,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>130</v>
       </c>
@@ -1839,7 +3507,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>92</v>
       </c>
@@ -1847,7 +3515,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>132</v>
       </c>
@@ -1855,7 +3523,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -1863,7 +3531,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>134</v>
       </c>
@@ -1871,7 +3539,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -1879,7 +3547,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>136</v>
       </c>
@@ -1887,7 +3555,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>138</v>
       </c>
@@ -1895,7 +3563,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>140</v>
       </c>
@@ -1903,7 +3571,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -1911,18 +3579,18 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>144</v>
       </c>
       <c r="B38" s="3"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="B39" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>146</v>
       </c>
@@ -1930,7 +3598,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -1938,7 +3606,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>150</v>
       </c>
@@ -1946,7 +3614,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -1954,7 +3622,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>154</v>
       </c>
@@ -1962,7 +3630,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>156</v>
       </c>
@@ -1970,7 +3638,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>158</v>
       </c>
@@ -1978,7 +3646,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>160</v>
       </c>
@@ -1986,7 +3654,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>162</v>
       </c>
@@ -1994,7 +3662,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2">
       <c r="B49" s="3" t="s">
         <v>164</v>
       </c>
@@ -2005,4 +3673,2230 @@
     <ignoredError sqref="B2:B49" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475247BC-66FE-4A74-AD0F-87C2108BF5ED}">
+  <dimension ref="A1:B276"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1">
+      <c r="A1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1">
+      <c r="A4" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" thickBot="1">
+      <c r="A5" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1">
+      <c r="A6" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" thickBot="1">
+      <c r="A7" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" thickBot="1">
+      <c r="A8" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" thickBot="1">
+      <c r="A9" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1">
+      <c r="A10" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" thickBot="1">
+      <c r="A11" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" thickBot="1">
+      <c r="A12" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1">
+      <c r="A13" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" thickBot="1">
+      <c r="A14" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" thickBot="1">
+      <c r="A15" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" thickBot="1">
+      <c r="A16" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1">
+      <c r="A17" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1">
+      <c r="A18" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickBot="1">
+      <c r="A19" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1">
+      <c r="A20" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" thickBot="1">
+      <c r="A21" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1">
+      <c r="A22" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" thickBot="1">
+      <c r="A23" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1">
+      <c r="A24" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15" thickBot="1">
+      <c r="A25" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1">
+      <c r="A26" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1">
+      <c r="A27" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B27" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickBot="1">
+      <c r="A28" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B28" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" thickBot="1">
+      <c r="A29" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B29" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickBot="1">
+      <c r="A30" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B30" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1">
+      <c r="A31" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1">
+      <c r="A32" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B32" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1">
+      <c r="A33" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B33" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1">
+      <c r="A34" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" thickBot="1">
+      <c r="A35" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B35" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1">
+      <c r="A36" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B36" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1">
+      <c r="A37" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" thickBot="1">
+      <c r="A38" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B38" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" thickBot="1">
+      <c r="A39" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" thickBot="1">
+      <c r="A40" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1">
+      <c r="A41" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" thickBot="1">
+      <c r="A42" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B42" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1">
+      <c r="A43" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" thickBot="1">
+      <c r="A44" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B44" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1">
+      <c r="A45" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B45" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" thickBot="1">
+      <c r="A46" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" thickBot="1">
+      <c r="A47" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B47" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" thickBot="1">
+      <c r="A48" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B48" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1">
+      <c r="A49" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B49" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" thickBot="1">
+      <c r="A50" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" thickBot="1">
+      <c r="A51" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B51" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" thickBot="1">
+      <c r="A52" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B52" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1">
+      <c r="A53" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" thickBot="1">
+      <c r="A54" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B54" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" thickBot="1">
+      <c r="A55" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B55" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" thickBot="1">
+      <c r="A56" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B56" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15" thickBot="1">
+      <c r="A57" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B57" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" thickBot="1">
+      <c r="A58" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B58" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1">
+      <c r="A59" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B59" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" thickBot="1">
+      <c r="A60" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B60" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" thickBot="1">
+      <c r="A61" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B61" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" thickBot="1">
+      <c r="A62" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B62" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15" thickBot="1">
+      <c r="A63" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B63" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" thickBot="1">
+      <c r="A64" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B64" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15" thickBot="1">
+      <c r="A65" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B65" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" thickBot="1">
+      <c r="A66" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B66" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15" thickBot="1">
+      <c r="A67" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B67" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15" thickBot="1">
+      <c r="A68" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B68" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15" thickBot="1">
+      <c r="A69" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B69" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15" thickBot="1">
+      <c r="A70" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B70" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15" thickBot="1">
+      <c r="A71" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B71" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15" thickBot="1">
+      <c r="A72" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B72" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15" thickBot="1">
+      <c r="A73" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B73" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15" thickBot="1">
+      <c r="A74" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B74" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15" thickBot="1">
+      <c r="A75" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B75" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15" thickBot="1">
+      <c r="A76" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B76" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15" thickBot="1">
+      <c r="A77" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B77" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15" thickBot="1">
+      <c r="A78" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B78" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15" thickBot="1">
+      <c r="A79" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B79" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15" thickBot="1">
+      <c r="A80" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B80" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15" thickBot="1">
+      <c r="A81" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B81" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15" thickBot="1">
+      <c r="A82" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B82" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15" thickBot="1">
+      <c r="A83" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B83" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15" thickBot="1">
+      <c r="A84" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B84" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15" thickBot="1">
+      <c r="A85" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B85" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15" thickBot="1">
+      <c r="A86" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B86" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15" thickBot="1">
+      <c r="A87" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B87" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15" thickBot="1">
+      <c r="A88" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B88" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15" thickBot="1">
+      <c r="A89" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B89" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" thickBot="1">
+      <c r="A90" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B90" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15" thickBot="1">
+      <c r="A91" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B91" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15" thickBot="1">
+      <c r="A92" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B92" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15" thickBot="1">
+      <c r="A93" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B93" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" thickBot="1">
+      <c r="A94" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B94" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" thickBot="1">
+      <c r="A95" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B95" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" thickBot="1">
+      <c r="A96" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B96" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15" thickBot="1">
+      <c r="A97" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B97" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15" thickBot="1">
+      <c r="A98" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B98" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15" thickBot="1">
+      <c r="A99" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B99" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15" thickBot="1">
+      <c r="A100" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B100" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15" thickBot="1">
+      <c r="A101" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B101" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15" thickBot="1">
+      <c r="A102" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B102" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15" thickBot="1">
+      <c r="A103" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B103" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15" thickBot="1">
+      <c r="A104" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B104" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15" thickBot="1">
+      <c r="A105" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B105" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15" thickBot="1">
+      <c r="A106" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B106" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15" thickBot="1">
+      <c r="A107" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B107" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15" thickBot="1">
+      <c r="A108" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B108" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="15" thickBot="1">
+      <c r="A109" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B109" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15" thickBot="1">
+      <c r="A110" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B110" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="15" thickBot="1">
+      <c r="A111" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B111" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="15" thickBot="1">
+      <c r="A112" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B112" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15" thickBot="1">
+      <c r="A113" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B113" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15" thickBot="1">
+      <c r="A114" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B114" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15" thickBot="1">
+      <c r="A115" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B115" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15" thickBot="1">
+      <c r="A116" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B116" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15" thickBot="1">
+      <c r="A117" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B117" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="15" thickBot="1">
+      <c r="A118" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B118" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="15" thickBot="1">
+      <c r="A119" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B119" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="15" thickBot="1">
+      <c r="A120" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B120" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="15" thickBot="1">
+      <c r="A121" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B121" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="15" thickBot="1">
+      <c r="A122" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B122" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="15" thickBot="1">
+      <c r="A123" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B123" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15" thickBot="1">
+      <c r="A124" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B124" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15" thickBot="1">
+      <c r="A125" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B125" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="15" thickBot="1">
+      <c r="A126" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B126" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15" thickBot="1">
+      <c r="A127" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B127" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="15" thickBot="1">
+      <c r="A128" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B128" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="15" thickBot="1">
+      <c r="A129" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B129" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15" thickBot="1">
+      <c r="A130" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B130" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15" thickBot="1">
+      <c r="A131" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B131" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15" thickBot="1">
+      <c r="A132" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B132" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15" thickBot="1">
+      <c r="A133" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B133" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15" thickBot="1">
+      <c r="A134" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B134" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15" thickBot="1">
+      <c r="A135" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B135" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15" thickBot="1">
+      <c r="A136" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B136" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15" thickBot="1">
+      <c r="A137" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B137" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15" thickBot="1">
+      <c r="A138" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B138" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15" thickBot="1">
+      <c r="A139" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B139" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15" thickBot="1">
+      <c r="A140" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B140" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15" thickBot="1">
+      <c r="A141" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B141" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15" thickBot="1">
+      <c r="A142" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B142" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15" thickBot="1">
+      <c r="A143" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B143" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15" thickBot="1">
+      <c r="A144" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B144" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15" thickBot="1">
+      <c r="A145" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B145" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15" thickBot="1">
+      <c r="A146" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B146" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15" thickBot="1">
+      <c r="A147" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B147" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15" thickBot="1">
+      <c r="A148" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B148" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="15" thickBot="1">
+      <c r="A149" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B149" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15" thickBot="1">
+      <c r="A150" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B150" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="15" thickBot="1">
+      <c r="A151" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B151" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="15" thickBot="1">
+      <c r="A152" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B152" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="15" thickBot="1">
+      <c r="A153" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B153" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="15" thickBot="1">
+      <c r="A154" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B154" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="15" thickBot="1">
+      <c r="A155" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B155" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="15" thickBot="1">
+      <c r="A156" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B156" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="15" thickBot="1">
+      <c r="A157" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="B157" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="15" thickBot="1">
+      <c r="A158" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B158" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="15" thickBot="1">
+      <c r="A159" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B159" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="15" thickBot="1">
+      <c r="A160" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B160" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="15" thickBot="1">
+      <c r="A161" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B161" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="15" thickBot="1">
+      <c r="A162" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B162" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="15" thickBot="1">
+      <c r="A163" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B163" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="15" thickBot="1">
+      <c r="A164" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B164" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15" thickBot="1">
+      <c r="A165" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B165" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="15" thickBot="1">
+      <c r="A166" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B166" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="15" thickBot="1">
+      <c r="A167" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B167" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="15" thickBot="1">
+      <c r="A168" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B168" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="15" thickBot="1">
+      <c r="A169" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B169" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="15" thickBot="1">
+      <c r="A170" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B170" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15" thickBot="1">
+      <c r="A171" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B171" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15" thickBot="1">
+      <c r="A172" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B172" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="15" thickBot="1">
+      <c r="A173" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B173" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15" thickBot="1">
+      <c r="A174" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B174" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="15" thickBot="1">
+      <c r="A175" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B175" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="15" thickBot="1">
+      <c r="A176" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="B176" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15" thickBot="1">
+      <c r="A177" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B177" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15" thickBot="1">
+      <c r="A178" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B178" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="15" thickBot="1">
+      <c r="A179" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B179" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15" thickBot="1">
+      <c r="A180" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B180" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="15" thickBot="1">
+      <c r="A181" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B181" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="15" thickBot="1">
+      <c r="A182" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B182" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="15" thickBot="1">
+      <c r="A183" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B183" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="15" thickBot="1">
+      <c r="A184" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B184" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="15" thickBot="1">
+      <c r="A185" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B185" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="15" thickBot="1">
+      <c r="A186" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B186" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15" thickBot="1">
+      <c r="A187" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B187" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="15" thickBot="1">
+      <c r="A188" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B188" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="15" thickBot="1">
+      <c r="A189" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B189" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="15" thickBot="1">
+      <c r="A190" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B190" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="15" thickBot="1">
+      <c r="A191" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B191" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="15" thickBot="1">
+      <c r="A192" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B192" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="15" thickBot="1">
+      <c r="A193" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="B193" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="15" thickBot="1">
+      <c r="A194" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B194" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15" thickBot="1">
+      <c r="A195" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B195" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15" thickBot="1">
+      <c r="A196" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B196" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="15" thickBot="1">
+      <c r="A197" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B197" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="15" thickBot="1">
+      <c r="A198" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B198" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15" thickBot="1">
+      <c r="A199" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B199" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="15" thickBot="1">
+      <c r="A200" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B200" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="15" thickBot="1">
+      <c r="A201" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="B201" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="15" thickBot="1">
+      <c r="A202" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B202" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="15" thickBot="1">
+      <c r="A203" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B203" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="15" thickBot="1">
+      <c r="A204" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B204" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="15" thickBot="1">
+      <c r="A205" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B205" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="15" thickBot="1">
+      <c r="A206" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B206" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="15" thickBot="1">
+      <c r="A207" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="B207" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="15" thickBot="1">
+      <c r="A208" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B208" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="15" thickBot="1">
+      <c r="A209" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B209" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="15" thickBot="1">
+      <c r="A210" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B210" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="15" thickBot="1">
+      <c r="A211" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B211" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="15" thickBot="1">
+      <c r="A212" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B212" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="15" thickBot="1">
+      <c r="A213" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B213" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="15" thickBot="1">
+      <c r="A214" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B214" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="15" thickBot="1">
+      <c r="A215" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B215" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="15" thickBot="1">
+      <c r="A216" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B216" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="15" thickBot="1">
+      <c r="A217" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B217" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="15" thickBot="1">
+      <c r="A218" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="B218" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="15" thickBot="1">
+      <c r="A219" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B219" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="15" thickBot="1">
+      <c r="A220" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B220" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="15" thickBot="1">
+      <c r="A221" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B221" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="15" thickBot="1">
+      <c r="A222" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B222" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="15" thickBot="1">
+      <c r="A223" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B223" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="15" thickBot="1">
+      <c r="A224" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B224" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="15" thickBot="1">
+      <c r="A225" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B225" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="15" thickBot="1">
+      <c r="A226" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="B226" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="15" thickBot="1">
+      <c r="A227" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B227" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="15" thickBot="1">
+      <c r="A228" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B228" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="15" thickBot="1">
+      <c r="A229" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B229" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="15" thickBot="1">
+      <c r="A230" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B230" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" ht="15" thickBot="1">
+      <c r="A231" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B231" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" ht="15" thickBot="1">
+      <c r="A232" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B232" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" ht="15" thickBot="1">
+      <c r="A233" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B233" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="15" thickBot="1">
+      <c r="A234" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B234" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="15" thickBot="1">
+      <c r="A235" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B235" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="15" thickBot="1">
+      <c r="A236" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="B236" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" ht="15" thickBot="1">
+      <c r="A237" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B237" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="15" thickBot="1">
+      <c r="A238" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="B238" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="15" thickBot="1">
+      <c r="A239" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B239" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="15" thickBot="1">
+      <c r="A240" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B240" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="15" thickBot="1">
+      <c r="A241" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B241" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" ht="15" thickBot="1">
+      <c r="A242" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B242" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" ht="15" thickBot="1">
+      <c r="A243" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B243" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="15" thickBot="1">
+      <c r="A244" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B244" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" ht="15" thickBot="1">
+      <c r="A245" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B245" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" ht="15" thickBot="1">
+      <c r="A246" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="B246" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" ht="15" thickBot="1">
+      <c r="A247" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B247" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="15" thickBot="1">
+      <c r="A248" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B248" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="15" thickBot="1">
+      <c r="A249" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B249" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="15" thickBot="1">
+      <c r="A250" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B250" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="15" thickBot="1">
+      <c r="A251" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B251" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="15" thickBot="1">
+      <c r="A252" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B252" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" ht="15" thickBot="1">
+      <c r="A253" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B253" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" ht="15" thickBot="1">
+      <c r="A254" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B254" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" ht="15" thickBot="1">
+      <c r="A255" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B255" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="15" thickBot="1">
+      <c r="A256" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B256" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="15" thickBot="1">
+      <c r="A257" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B257" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="15" thickBot="1">
+      <c r="A258" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B258" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" ht="15" thickBot="1">
+      <c r="A259" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B259" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="15" thickBot="1">
+      <c r="A260" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B260" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="15" thickBot="1">
+      <c r="A261" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B261" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="15" thickBot="1">
+      <c r="A262" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B262" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="15" thickBot="1">
+      <c r="A263" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B263" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" ht="15" thickBot="1">
+      <c r="A264" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="B264" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="15" thickBot="1">
+      <c r="A265" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B265" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="15" thickBot="1">
+      <c r="A266" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B266" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="15" thickBot="1">
+      <c r="A267" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B267" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="15" thickBot="1">
+      <c r="A268" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B268" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="15" thickBot="1">
+      <c r="A269" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B269" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="15" thickBot="1">
+      <c r="A270" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="B270" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="15" thickBot="1">
+      <c r="A271" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="B271" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="15" thickBot="1">
+      <c r="A272" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B272" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="15" thickBot="1">
+      <c r="A273" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="B273" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="15" thickBot="1">
+      <c r="A274" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B274" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="15" thickBot="1">
+      <c r="A275" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="B275" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="15" thickBot="1">
+      <c r="A276" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B276" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>